<commit_message>
now keeping track of best unit in a lap, but continuing with a random one.  Added 2 new csv files to help with tracking information
</commit_message>
<xml_diff>
--- a/MicroRTS/Results.xlsx
+++ b/MicroRTS/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kynan\Documents\MicroRTS_Research\MicroRTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138AC9AD-05A5-42EF-9EFD-131F0B6F7006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4B42E-D613-4902-AC2A-311C0A0D1B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawResults#1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="RawResults#3" sheetId="6" r:id="rId6"/>
     <sheet name="BestResults#4" sheetId="7" r:id="rId7"/>
     <sheet name="RawResults#4" sheetId="8" r:id="rId8"/>
+    <sheet name="RawResults#5" sheetId="9" r:id="rId9"/>
+    <sheet name="BestResults#5" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="489">
   <si>
     <t>Killer has cost: 3 hp: 1 min Damage: 1 max Damage: 1 attack range: 2</t>
   </si>
@@ -1376,6 +1378,129 @@
   </si>
   <si>
     <t>Killer has cost: 4 hp: 3 max Damage: 1 attack range: 1 move speed: 5 attack speed: 1</t>
+  </si>
+  <si>
+    <t>Killer has cost: 4 hp: 3 min Damage: 1 max Damage: 1 attack range: 1</t>
+  </si>
+  <si>
+    <t>The score was: 0.05158371</t>
+  </si>
+  <si>
+    <t>The score was: 0.06735747</t>
+  </si>
+  <si>
+    <t>The score was: 0.02704026</t>
+  </si>
+  <si>
+    <t>The score was: 0.0</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 2 max Damage: 2 attack range: 1</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 1 max Damage: 2 attack range: 1</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 0 max Damage: 1 attack range: 1</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 0 max Damage: 0 attack range: 1</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 1 max Damage: 1 attack range: 2</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 3 min Damage: 1 max Damage: 1 attack range: 1</t>
+  </si>
+  <si>
+    <t>The score was: 0.016931217</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 3 move speed: 11 attack speed: 1</t>
+  </si>
+  <si>
+    <t>The total score was : 1.2708803</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: 0.27088037</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 2 move speed: 11 attack speed: 1</t>
+  </si>
+  <si>
+    <t>The total score was : 1.0364103</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: 0.20307693</t>
+  </si>
+  <si>
+    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 2 move speed: 6 attack speed: 1</t>
+  </si>
+  <si>
+    <t>The total score was : 1.3181102</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: 0.31811023</t>
+  </si>
+  <si>
+    <t>Killer has cost: 1 hp: 4 max Damage: 2 attack range: 1 move speed: 14 attack speed: 1</t>
+  </si>
+  <si>
+    <t>The total score was : 0.464634</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: -0.535366</t>
+  </si>
+  <si>
+    <t>The unit was made in and was won with in : 3 games</t>
+  </si>
+  <si>
+    <t>The unit was made by player 0 in: 7 games</t>
+  </si>
+  <si>
+    <t>The unit was made by player 1 in: 5 games</t>
+  </si>
+  <si>
+    <t>The unit was made by both players in the same game in: 4 games</t>
+  </si>
+  <si>
+    <t>The unit was made in and was won with by player 0 in : 4 games</t>
+  </si>
+  <si>
+    <t>The unit was made in and was won with by player 1 in : 4 games</t>
+  </si>
+  <si>
+    <t>The total score was : 1.2068771</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: 0.20687713</t>
+  </si>
+  <si>
+    <t>The unit was made in: 6 games</t>
+  </si>
+  <si>
+    <t>The unit was made in and was won with in : 2 games</t>
+  </si>
+  <si>
+    <t>The unit was made by player 1 in: 9 games</t>
+  </si>
+  <si>
+    <t>The unit was made by both players in the same game in: 8 games</t>
+  </si>
+  <si>
+    <t>The total score was : 0.96403915</t>
+  </si>
+  <si>
+    <t>The score for round 1 was: 0.03546777</t>
+  </si>
+  <si>
+    <t>The score for round 2 was: 0.9285714</t>
+  </si>
+  <si>
+    <t>The unit was made by player 1 in: 6 games</t>
+  </si>
+  <si>
+    <t>The unit was made by both players in the same game in: 5 games</t>
   </si>
 </sst>
 </file>
@@ -4206,6 +4331,588 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A4D7C0-11F0-41BA-A74D-1375242FD1A8}">
+  <dimension ref="B2:C109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E26F2B5-51B9-495C-AC20-3ECA3EAA804B}">
   <dimension ref="A2:B51"/>
@@ -15619,8 +16326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC25D70-3130-4793-A7BF-B10878254699}">
   <dimension ref="A2:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15903,4 +16610,254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA44A1BE-C14F-42B8-BCB9-D44AD8C1A5C5}">
+  <dimension ref="A2:A48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished adding cause and effects, and updated how the results are reported for ease of use in excel.  other minor fixes
</commit_message>
<xml_diff>
--- a/MicroRTS/Results.xlsx
+++ b/MicroRTS/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kynan\Documents\MicroRTS_Research\MicroRTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4B42E-D613-4902-AC2A-311C0A0D1B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC99302-7B15-43F8-9CCF-9CF886CC23E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31665" yWindow="1800" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawResults#1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="460">
   <si>
     <t>Killer has cost: 3 hp: 1 min Damage: 1 max Damage: 1 attack range: 2</t>
   </si>
@@ -1414,93 +1414,6 @@
   </si>
   <si>
     <t>The score was: 0.016931217</t>
-  </si>
-  <si>
-    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 3 move speed: 11 attack speed: 1</t>
-  </si>
-  <si>
-    <t>The total score was : 1.2708803</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: 0.27088037</t>
-  </si>
-  <si>
-    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 2 move speed: 11 attack speed: 1</t>
-  </si>
-  <si>
-    <t>The total score was : 1.0364103</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: 0.20307693</t>
-  </si>
-  <si>
-    <t>Killer has cost: 3 hp: 4 max Damage: 1 attack range: 2 move speed: 6 attack speed: 1</t>
-  </si>
-  <si>
-    <t>The total score was : 1.3181102</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: 0.31811023</t>
-  </si>
-  <si>
-    <t>Killer has cost: 1 hp: 4 max Damage: 2 attack range: 1 move speed: 14 attack speed: 1</t>
-  </si>
-  <si>
-    <t>The total score was : 0.464634</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: -0.535366</t>
-  </si>
-  <si>
-    <t>The unit was made in and was won with in : 3 games</t>
-  </si>
-  <si>
-    <t>The unit was made by player 0 in: 7 games</t>
-  </si>
-  <si>
-    <t>The unit was made by player 1 in: 5 games</t>
-  </si>
-  <si>
-    <t>The unit was made by both players in the same game in: 4 games</t>
-  </si>
-  <si>
-    <t>The unit was made in and was won with by player 0 in : 4 games</t>
-  </si>
-  <si>
-    <t>The unit was made in and was won with by player 1 in : 4 games</t>
-  </si>
-  <si>
-    <t>The total score was : 1.2068771</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: 0.20687713</t>
-  </si>
-  <si>
-    <t>The unit was made in: 6 games</t>
-  </si>
-  <si>
-    <t>The unit was made in and was won with in : 2 games</t>
-  </si>
-  <si>
-    <t>The unit was made by player 1 in: 9 games</t>
-  </si>
-  <si>
-    <t>The unit was made by both players in the same game in: 8 games</t>
-  </si>
-  <si>
-    <t>The total score was : 0.96403915</t>
-  </si>
-  <si>
-    <t>The score for round 1 was: 0.03546777</t>
-  </si>
-  <si>
-    <t>The score for round 2 was: 0.9285714</t>
-  </si>
-  <si>
-    <t>The unit was made by player 1 in: 6 games</t>
-  </si>
-  <si>
-    <t>The unit was made by both players in the same game in: 5 games</t>
   </si>
 </sst>
 </file>
@@ -4333,582 +4246,14 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A4D7C0-11F0-41BA-A74D-1375242FD1A8}">
-  <dimension ref="B2:C109"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C109"/>
+      <selection activeCell="I8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>49</v>
-      </c>
-      <c r="C62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>43</v>
-      </c>
-      <c r="C74" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>45</v>
-      </c>
-      <c r="C86" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>46</v>
-      </c>
-      <c r="C98" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>